<commit_message>
minor amendments in main_page set up
</commit_message>
<xml_diff>
--- a/WASH_shiny1.xlsx
+++ b/WASH_shiny1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/plhR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{0EF9535E-66F1-4870-9078-2E60F5A89791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76419A5E-A499-443A-8093-0D2B59731263}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7797F92C-659C-4C0C-93ED-C02A99145971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="150">
   <si>
     <t>type</t>
   </si>
@@ -460,58 +460,25 @@
     <t>myvaluebox3</t>
   </si>
   <si>
-    <t>text = "Completed Onboarding", colour = "aqua", icon = "check"</t>
-  </si>
-  <si>
-    <t>completed_onboarding</t>
-  </si>
-  <si>
-    <t>myvaluebox4</t>
-  </si>
-  <si>
-    <t>text = "Active in last 24 hours", colour = "green", icon = "clock"</t>
-  </si>
-  <si>
-    <t>active_in_last_24_hours</t>
-  </si>
-  <si>
-    <t>myvaluebox5</t>
-  </si>
-  <si>
-    <t>text = "Active in last 7 days", colour = "orange", icon = "calendar"</t>
-  </si>
-  <si>
-    <t>active_in_last_7_days</t>
-  </si>
-  <si>
     <t>mean_box</t>
   </si>
   <si>
-    <t>myvaluebox6</t>
-  </si>
-  <si>
     <t>text = "Average days in the chatbot", colour = "orange", icon = "active"</t>
   </si>
   <si>
     <t>time_in_study_n</t>
   </si>
   <si>
-    <t>perc_goals_completed</t>
-  </si>
-  <si>
-    <t>perc_modules_completed</t>
-  </si>
-  <si>
-    <t>myvaluebox7</t>
-  </si>
-  <si>
-    <t>myvaluebox8</t>
-  </si>
-  <si>
-    <t>text = "Average goals completed (%)", colour = "aqua", icon = "bullseye"</t>
-  </si>
-  <si>
-    <t>text = "Average modules completed (%)", colour = "purple", icon = "star"</t>
+    <t>checkbox_group</t>
+  </si>
+  <si>
+    <t>label = "User Enrolled", choices = c("yes", "no"), selected = c("yes", "no")</t>
+  </si>
+  <si>
+    <t>checkboxfilter1</t>
+  </si>
+  <si>
+    <t>filter_box</t>
   </si>
 </sst>
 </file>
@@ -609,10 +576,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1077,16 +1040,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42C664-DDE1-4EE9-A709-5E4583FEC77F}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D521C-A218-4630-A92D-9512A3F85D41}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="67.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1094,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1114,6 +1082,9 @@
         <v>134</v>
       </c>
       <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
         <v>135</v>
       </c>
       <c r="D2" t="s">
@@ -1131,6 +1102,9 @@
         <v>134</v>
       </c>
       <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
         <v>138</v>
       </c>
       <c r="D3" t="s">
@@ -1148,97 +1122,38 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
         <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1247,7 +1162,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1255,6 +1170,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
type == "box" implementation
</commit_message>
<xml_diff>
--- a/WASH_shiny1.xlsx
+++ b/WASH_shiny1.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7797F92C-659C-4C0C-93ED-C02A99145971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2EB7C1-07D3-4726-8893-37C07FF1C00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" tabRatio="935" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
     <sheet name="main_page" sheetId="16" r:id="rId2"/>
     <sheet name="demographics" sheetId="1" r:id="rId3"/>
     <sheet name="td_engagement" sheetId="10" r:id="rId4"/>
-    <sheet name="td_eng_completed" sheetId="9" r:id="rId5"/>
-    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId6"/>
-    <sheet name="td_eng_started" sheetId="11" r:id="rId7"/>
-    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId8"/>
-    <sheet name="td_modules" sheetId="14" r:id="rId9"/>
+    <sheet name="td_modules" sheetId="14" r:id="rId5"/>
+    <sheet name="td_eng_completed" sheetId="9" r:id="rId6"/>
+    <sheet name="td_eng_completed_toggle" sheetId="13" r:id="rId7"/>
+    <sheet name="td_eng_started" sheetId="11" r:id="rId8"/>
+    <sheet name="td_eng_started_toggle" sheetId="12" r:id="rId9"/>
     <sheet name="td_modules_started" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="151">
   <si>
     <t>type</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>filter_box</t>
+  </si>
+  <si>
+    <t>box</t>
   </si>
 </sst>
 </file>
@@ -867,9 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -937,14 +938,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF59F33-DB76-4BC9-93A0-DA4FB6A22DCC}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -952,7 +956,7 @@
     <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,13 +985,16 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" t="s">
         <v>126</v>
       </c>
@@ -1007,13 +1014,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" t="s">
         <v>129</v>
       </c>
@@ -1032,6 +1042,21 @@
       <c r="I3" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1043,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D521C-A218-4630-A92D-9512A3F85D41}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1199,11 +1224,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
@@ -1216,16 +1244,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1233,16 +1264,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -1250,11 +1284,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
@@ -1267,10 +1304,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -1361,11 +1401,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DAF98-772F-4DFA-8572-31F09E1E6A1F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1400,11 +1475,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" t="s">
         <v>39</v>
       </c>
@@ -1417,11 +1495,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" t="s">
         <v>40</v>
       </c>
@@ -1434,11 +1515,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
@@ -1451,11 +1535,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>42</v>
       </c>
@@ -1468,11 +1555,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
         <v>43</v>
       </c>
@@ -1485,11 +1575,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
@@ -1502,11 +1595,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
@@ -1519,11 +1615,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" t="s">
         <v>46</v>
       </c>
@@ -1536,11 +1635,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>47</v>
       </c>
@@ -1553,11 +1655,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" t="s">
         <v>48</v>
       </c>
@@ -1570,11 +1675,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
@@ -1587,10 +1695,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>50</v>
@@ -1608,12 +1719,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1CC97C-CAD1-465E-AE96-2C034F6B7FC0}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,11 +1754,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" t="s">
         <v>39</v>
       </c>
@@ -1660,11 +1774,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" t="s">
         <v>40</v>
       </c>
@@ -1677,11 +1794,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
@@ -1694,11 +1814,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>42</v>
       </c>
@@ -1711,11 +1834,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
         <v>43</v>
       </c>
@@ -1728,11 +1854,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
@@ -1745,11 +1874,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
@@ -1762,11 +1894,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" t="s">
         <v>46</v>
       </c>
@@ -1779,11 +1914,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>47</v>
       </c>
@@ -1796,11 +1934,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" t="s">
         <v>48</v>
       </c>
@@ -1813,11 +1954,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
@@ -1830,10 +1974,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>50</v>
@@ -1850,12 +1997,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF14D57-0BE2-4D81-A4A6-F122E72BED91}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1885,11 +2032,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" t="s">
         <v>55</v>
       </c>
@@ -1902,11 +2052,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" t="s">
         <v>56</v>
       </c>
@@ -1919,11 +2072,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
@@ -1936,11 +2092,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>58</v>
       </c>
@@ -1953,11 +2112,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
         <v>59</v>
       </c>
@@ -1970,11 +2132,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" t="s">
         <v>60</v>
       </c>
@@ -1987,11 +2152,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
@@ -2004,11 +2172,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" t="s">
         <v>62</v>
       </c>
@@ -2021,11 +2192,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>63</v>
       </c>
@@ -2038,11 +2212,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
@@ -2055,11 +2232,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
@@ -2072,10 +2252,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
@@ -2093,12 +2276,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80786C0-93AB-482A-9BF1-EF3E9BEE8E3A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2128,11 +2311,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" t="s">
         <v>55</v>
       </c>
@@ -2145,11 +2331,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" t="s">
         <v>56</v>
       </c>
@@ -2162,11 +2351,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
@@ -2179,11 +2371,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>58</v>
       </c>
@@ -2196,11 +2391,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
         <v>59</v>
       </c>
@@ -2213,11 +2411,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" t="s">
         <v>60</v>
       </c>
@@ -2230,11 +2431,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
@@ -2247,11 +2451,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" t="s">
         <v>62</v>
       </c>
@@ -2264,11 +2471,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>63</v>
       </c>
@@ -2281,11 +2491,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
@@ -2298,11 +2511,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
@@ -2315,11 +2531,14 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" t="s">
         <v>66</v>
       </c>
@@ -2328,41 +2547,6 @@
       </c>
       <c r="G13">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137D2B-4CCD-4240-B497-71AEC5867C95}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>